<commit_message>
Corrección muestreo de datos Sucursales
</commit_message>
<xml_diff>
--- a/SpaOnline/ModeloDominio/Sucursales - Muestreo Datos .xlsx
+++ b/SpaOnline/ModeloDominio/Sucursales - Muestreo Datos .xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grchia-my.sharepoint.com/personal/jhonatan_gomez_wiga_io/Documents/Escritorio/UCO/DOO/SpaOnline/ModeloDominio/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DOO\DOO\SpaOnline\ModeloDominio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{B9D1E950-751B-4E46-9074-9E1B23E2FD1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{656693FD-15D8-44DE-9459-28B9B23A97A4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EF57805-8B1C-4531-8E23-0C94A0E91C20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="5" xr2:uid="{9AD29915-CB49-430C-A10E-F60FF2C9A65A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="7" xr2:uid="{9AD29915-CB49-430C-A10E-F60FF2C9A65A}"/>
   </bookViews>
   <sheets>
     <sheet name="Modelo de Dominio Anemico" sheetId="1" r:id="rId1"/>
@@ -18,8 +18,8 @@
     <sheet name="Pais" sheetId="6" r:id="rId3"/>
     <sheet name="Departamento" sheetId="7" r:id="rId4"/>
     <sheet name="Ciudad" sheetId="8" r:id="rId5"/>
-    <sheet name="Sucursal" sheetId="5" r:id="rId6"/>
-    <sheet name="Instituciones" sheetId="9" r:id="rId7"/>
+    <sheet name="Spa" sheetId="9" r:id="rId6"/>
+    <sheet name="Sucursal" sheetId="5" r:id="rId7"/>
     <sheet name="Agenda" sheetId="10" r:id="rId8"/>
   </sheets>
   <externalReferences>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="65">
   <si>
     <t xml:space="preserve">Nombre </t>
   </si>
@@ -161,9 +161,6 @@
     <t xml:space="preserve">Objeto de domino que contiene el nombre de las ciudades  que pertenecen a un departamento determinado </t>
   </si>
   <si>
-    <t xml:space="preserve">Objeto de domino que representa cada uno de los tipos de identificacion tributaria de los negocios en un pais </t>
-  </si>
-  <si>
     <t>Direccion</t>
   </si>
   <si>
@@ -194,9 +191,6 @@
     <t>Referenciado</t>
   </si>
   <si>
-    <t>Instituciones</t>
-  </si>
-  <si>
     <t>Institucion</t>
   </si>
   <si>
@@ -218,9 +212,6 @@
     <t>SpaOnline</t>
   </si>
   <si>
-    <t>SpaManitas</t>
-  </si>
-  <si>
     <t>HorariosAtencion</t>
   </si>
   <si>
@@ -263,7 +254,13 @@
     <t>Agenda</t>
   </si>
   <si>
-    <t>Objeto de domino que representa la Disponibilidad de la sucursal para agendar las reservas</t>
+    <t>Spa</t>
+  </si>
+  <si>
+    <t>Objeto de domino que contiene la información del spa y del personal</t>
+  </si>
+  <si>
+    <t>Objeto de domino que representa la disponibilidad de la sucursal para agendar las reservas</t>
   </si>
 </sst>
 </file>
@@ -369,7 +366,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -404,6 +401,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -432,17 +430,17 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>544064</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>57690</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>189596</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>28801</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Imagen 3">
+        <xdr:cNvPr id="2" name="Imagen 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69A29705-1825-9C5D-0750-8C5A29556DEF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C97E6E1-035E-063E-2DF2-516A1265A005}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -459,7 +457,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="8164064" cy="3867690"/>
+          <a:ext cx="10793331" cy="4906060"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -480,15 +478,15 @@
     <sheetNames>
       <sheetName val="Modelo de Dominio Anemico"/>
       <sheetName val="Objetos de dominio"/>
-      <sheetName val="Institucion"/>
+      <sheetName val="Spa"/>
       <sheetName val="Trabajador"/>
       <sheetName val="Administrador"/>
       <sheetName val="TipoIdentificacion"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
       <sheetData sheetId="3">
         <row r="2">
           <cell r="B2" t="str">
@@ -503,11 +501,6 @@
         <row r="4">
           <cell r="B4" t="str">
             <v>Luis Ospina</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="B5" t="str">
-            <v>Juan Pablo Rendon Gómez</v>
           </cell>
         </row>
       </sheetData>
@@ -875,8 +868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA198BEE-AB41-4447-8B76-5672FB9C01F4}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView topLeftCell="A2" zoomScale="83" workbookViewId="0">
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -894,7 +887,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -977,10 +970,10 @@
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>65</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>3</v>
@@ -989,18 +982,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>31</v>
+        <v>63</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1010,6 +1003,7 @@
     <hyperlink ref="A4" location="Departamento!A1" display="Departamento" xr:uid="{5D026B1D-2A71-48AE-98F7-6FB6CEFAF94D}"/>
     <hyperlink ref="A5" location="Ciudad!A1" display="Ciudad" xr:uid="{3DB588EF-D6FF-42B3-9C3C-3D065A0B0817}"/>
     <hyperlink ref="A7" location="TipoIdentificacion!A1" display="TipoIdentificacion" xr:uid="{91E801FD-E3D2-4D3E-A38E-3A408F0036DE}"/>
+    <hyperlink ref="A6" location="Agenda!A1" display="Agenda" xr:uid="{9023DA42-6D23-4E2B-9D0C-BD687D7D068B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -1020,7 +1014,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CD8CC05-D5A5-4217-82D6-119F47E099F6}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1282,12 +1278,119 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EA2969B-FD1B-4144-8E9C-71E2B5D0B86A}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="1">
+        <v>900811919</v>
+      </c>
+      <c r="D2" s="20" t="str">
+        <f>[1]TipoIdentificacion!$B$3</f>
+        <v>NIT</v>
+      </c>
+      <c r="E2" s="20" t="str">
+        <f>[1]Administrador!B2</f>
+        <v xml:space="preserve">Jhoana Andrea Gómez Gómez </v>
+      </c>
+      <c r="F2" s="1" t="str">
+        <f>[1]Trabajador!B2</f>
+        <v xml:space="preserve">Jhonatan Arley Gómez </v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="1">
+        <v>900811919</v>
+      </c>
+      <c r="D3" s="20" t="str">
+        <f>[1]TipoIdentificacion!$B$3</f>
+        <v>NIT</v>
+      </c>
+      <c r="E3" s="20" t="str">
+        <f>[1]Administrador!B3</f>
+        <v>Nathaly perez Zapata</v>
+      </c>
+      <c r="F3" s="1" t="str">
+        <f>[1]Trabajador!B3</f>
+        <v>Cristian David Ospina Ospina</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="1">
+        <v>900811919</v>
+      </c>
+      <c r="D4" s="20" t="str">
+        <f>[1]TipoIdentificacion!$B$3</f>
+        <v>NIT</v>
+      </c>
+      <c r="E4" s="20" t="str">
+        <f>[1]Administrador!B4</f>
+        <v xml:space="preserve">Camilo Saldarriaga </v>
+      </c>
+      <c r="F4" s="1" t="str">
+        <f>[1]Trabajador!B4</f>
+        <v>Luis Ospina</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{952BDDC5-1485-4BC4-A31B-18839936F54D}">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1307,7 +1410,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>17</v>
@@ -1316,22 +1419,22 @@
         <v>7</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>37</v>
-      </c>
       <c r="H1" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>15</v>
       </c>
       <c r="J1" s="14" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -1339,11 +1442,11 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="str">
-        <f>Instituciones!B2</f>
+        <f>Spa!B2</f>
         <v>SpaOnline</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D2" s="13" t="str">
         <f>Ciudad!E2</f>
@@ -1353,13 +1456,13 @@
         <v>13</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G2" s="1">
         <v>54323243</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="I2" s="5" t="str">
         <f>D2&amp;"-"&amp;E2</f>
@@ -1375,11 +1478,11 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="str">
-        <f>Instituciones!B2</f>
+        <f>Spa!B2</f>
         <v>SpaOnline</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3" s="13" t="str">
         <f>Ciudad!E3</f>
@@ -1389,13 +1492,13 @@
         <v>12</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G3" s="1">
         <v>3214321</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="I3" s="5" t="str">
         <f t="shared" ref="I3:I4" si="0">D3&amp;"-"&amp;E3</f>
@@ -1411,11 +1514,11 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="str">
-        <f>Instituciones!B2</f>
+        <f>Spa!B2</f>
         <v>SpaOnline</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D4" s="13" t="str">
         <f>Ciudad!E4</f>
@@ -1425,13 +1528,13 @@
         <v>14</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G4" s="1">
         <v>5632421</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="I4" s="5" t="str">
         <f t="shared" si="0"/>
@@ -1462,98 +1565,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EA2969B-FD1B-4144-8E9C-71E2B5D0B86A}">
-  <dimension ref="A1:F3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="47.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="1">
-        <v>900811919</v>
-      </c>
-      <c r="D2" s="1" t="str">
-        <f>[1]TipoIdentificacion!B3</f>
-        <v>NIT</v>
-      </c>
-      <c r="E2" s="1" t="str">
-        <f>[1]Administrador!B2&amp;"-"&amp;[1]Administrador!B3</f>
-        <v>Jhoana Andrea Gómez Gómez -Nathaly perez Zapata</v>
-      </c>
-      <c r="F2" s="2" t="str">
-        <f>[1]Trabajador!B2&amp;"-"&amp;[1]Trabajador!B3&amp;"-"&amp;[1]Trabajador!B4</f>
-        <v>Jhonatan Arley Gómez -Cristian David Ospina Ospina-Luis Ospina</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C3" s="1">
-        <v>811912382</v>
-      </c>
-      <c r="D3" s="1" t="str">
-        <f>[1]TipoIdentificacion!B3</f>
-        <v>NIT</v>
-      </c>
-      <c r="E3" s="1" t="str">
-        <f>[1]Administrador!B4</f>
-        <v xml:space="preserve">Camilo Saldarriaga </v>
-      </c>
-      <c r="F3" s="1" t="str">
-        <f>[1]Trabajador!B5</f>
-        <v>Juan Pablo Rendon Gómez</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{084951A6-DA5B-432E-8D4D-0B97AEC0152B}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1570,13 +1587,13 @@
         <v>4</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>15</v>
@@ -1587,13 +1604,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E2" s="5" t="str">
         <f>C2&amp;"-"&amp;D2&amp;"-"&amp;B2</f>
@@ -1605,13 +1622,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E3" s="5" t="str">
         <f>C3&amp;"-"&amp;D3&amp;"-"&amp;B3</f>
@@ -1623,13 +1640,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E4" s="5" t="str">
         <f>C4&amp;"-"&amp;D4&amp;"-"&amp;B4</f>

</xml_diff>